<commit_message>
added Instruments as a component that can be created via factory
</commit_message>
<xml_diff>
--- a/doc/uml-diagrams/slot-properties.xlsx
+++ b/doc/uml-diagrams/slot-properties.xlsx
@@ -129,9 +129,6 @@
     <t>useOwnHeadingOnly</t>
   </si>
   <si>
-    <t>Physical gimbal type: "mechanical" or "electronic" (default: ELECTRONIC)</t>
-  </si>
-  <si>
     <t>Relative location vector (meters) [ x y z ] (default: 0,0,0)</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>Gain (default: 1.0)              (no units)</t>
+  </si>
+  <si>
+    <t>Physical identifiers: { mechanical, electronic } (default: electric)</t>
   </si>
 </sst>
 </file>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,13 +715,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -729,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -857,7 +857,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>23</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -929,15 +929,15 @@
         <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>30</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -977,15 +977,15 @@
         <v>32</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
         <v>33</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>34</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>35</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,152 +1017,152 @@
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
         <v>76</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" t="s">
         <v>99</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>